<commit_message>
refactor data wrangling functions
</commit_message>
<xml_diff>
--- a/data/demo.xlsx
+++ b/data/demo.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\initi\Development\ranking\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{0F5378A2-2AA7-4F21-A531-60C207AF8BE1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A037530-D338-4316-A0A8-C3AC03B3A47F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="demo_dummy" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -999,14 +999,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -1070,7 +1073,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>43102</v>
+        <v>42737</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -1092,7 +1095,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="1">
-        <v>43163</v>
+        <v>42798</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -1103,7 +1106,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>43321</v>
+        <v>42956</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -1114,7 +1117,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="1">
-        <v>43416</v>
+        <v>43051</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -1136,7 +1139,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="1">
-        <v>43103</v>
+        <v>42738</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -1147,7 +1150,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="1">
-        <v>43447</v>
+        <v>43082</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -1180,7 +1183,7 @@
         <v>13</v>
       </c>
       <c r="C15" s="1">
-        <v>43135</v>
+        <v>42770</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
@@ -1213,7 +1216,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="1">
-        <v>43164</v>
+        <v>42799</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1235,7 +1238,7 @@
         <v>18</v>
       </c>
       <c r="C20" s="1">
-        <v>43226</v>
+        <v>42861</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1246,7 +1249,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="1">
-        <v>43195</v>
+        <v>42830</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1268,7 +1271,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="1">
-        <v>43290</v>
+        <v>42925</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1279,7 +1282,7 @@
         <v>22</v>
       </c>
       <c r="C24" s="1">
-        <v>43322</v>
+        <v>42957</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1312,7 +1315,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="1">
-        <v>43224</v>
+        <v>42859</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1323,7 +1326,7 @@
         <v>26</v>
       </c>
       <c r="C28" s="1">
-        <v>43350</v>
+        <v>42985</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1356,7 +1359,7 @@
         <v>29</v>
       </c>
       <c r="C31" s="1">
-        <v>43213</v>
+        <v>42848</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1367,7 +1370,7 @@
         <v>30</v>
       </c>
       <c r="C32" s="1">
-        <v>43206</v>
+        <v>42841</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>